<commit_message>
Trying to figure out how temperature affects different parameters
</commit_message>
<xml_diff>
--- a/Varying Temperature Parameters.xlsx
+++ b/Varying Temperature Parameters.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livemanchesterac-my.sharepoint.com/personal/frederick_barrett_student_manchester_ac_uk/Documents/4th_Year/Dissertation/Main Project/Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{5E0AFF74-FA83-45EA-975A-7869487DBCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2C5AA05-D0A7-4707-80FF-A9F5DA59E12E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C654B8F6-E48E-4FC5-A85A-A6586FB73A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57675" yWindow="8190" windowWidth="15210" windowHeight="9495" xr2:uid="{922E80F0-49B4-4B8E-8D13-E35FB284D0A8}"/>
+    <workbookView xWindow="32415" yWindow="15990" windowWidth="25140" windowHeight="15915" xr2:uid="{922E80F0-49B4-4B8E-8D13-E35FB284D0A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Variable Parameters for Temperature sensitivity</t>
   </si>
@@ -144,6 +145,33 @@
   </si>
   <si>
     <t>Different temps will cause different max growth rates so I should find new values for these</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charge Transfer Coefficients </t>
+  </si>
+  <si>
+    <t>Dependent on temperature, I reckon I can say that everything else stays constant</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Values shown here for reference, in the code I will set up a direct relationship</t>
+  </si>
+  <si>
+    <t>Eg alpha = T/303*0.051 so I don't have to add data matrices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These are references for standard conditions and therefore do not need to be changed </t>
   </si>
 </sst>
 </file>
@@ -227,6 +255,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3200400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1257300</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>122811</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{990184F1-BEF8-B7C8-A796-A051FCC69B72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3810000" y="4229100"/>
+          <a:ext cx="5457825" cy="4180461"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -526,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E23C82-6B3B-441E-A6C1-C1E177A858BF}">
-  <dimension ref="B2:F20"/>
+  <dimension ref="B2:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -539,7 +616,10 @@
     <col min="3" max="3" width="9.140625" style="2"/>
     <col min="4" max="4" width="38.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="12" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
@@ -574,6 +654,9 @@
       <c r="E8" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="F8" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="9" spans="2:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
@@ -687,7 +770,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
@@ -704,12 +787,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>25</v>
       </c>
@@ -720,7 +803,405 @@
         <v>8.3299999999999997E-4</v>
       </c>
     </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G25" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G27" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F33" s="2">
+        <v>277</v>
+      </c>
+      <c r="G33" s="2">
+        <f>F33/$F$59*$G$59</f>
+        <v>4.6623762376237617E-2</v>
+      </c>
+      <c r="H33" s="2">
+        <f>F33/$F$59*$H$59</f>
+        <v>0.60610891089108909</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F34" s="2">
+        <v>278</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" ref="G34:G58" si="0">F34/$F$59*$G$59</f>
+        <v>4.6792079207920792E-2</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" ref="H34:H58" si="1">F34/$F$59*$H$59</f>
+        <v>0.60829702970297028</v>
+      </c>
+    </row>
+    <row r="35" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F35" s="2">
+        <v>279</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="0"/>
+        <v>4.696039603960396E-2</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="1"/>
+        <v>0.61048514851485158</v>
+      </c>
+    </row>
+    <row r="36" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F36" s="2">
+        <v>280</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7128712871287122E-2</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="1"/>
+        <v>0.61267326732673266</v>
+      </c>
+    </row>
+    <row r="37" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F37" s="2">
+        <v>281</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7297029702970297E-2</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="1"/>
+        <v>0.61486138613861385</v>
+      </c>
+    </row>
+    <row r="38" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F38" s="2">
+        <v>282</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7465346534653466E-2</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="1"/>
+        <v>0.61704950495049515</v>
+      </c>
+    </row>
+    <row r="39" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F39" s="2">
+        <v>283</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7633663366336627E-2</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="1"/>
+        <v>0.61923762376237623</v>
+      </c>
+    </row>
+    <row r="40" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F40" s="2">
+        <v>284</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7801980198019803E-2</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="1"/>
+        <v>0.62142574257425742</v>
+      </c>
+    </row>
+    <row r="41" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F41" s="2">
+        <v>285</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7970297029702964E-2</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.62361386138613861</v>
+      </c>
+    </row>
+    <row r="42" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F42" s="2">
+        <v>286</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="0"/>
+        <v>4.8138613861386133E-2</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="1"/>
+        <v>0.6258019801980198</v>
+      </c>
+    </row>
+    <row r="43" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F43" s="2">
+        <v>287</v>
+      </c>
+      <c r="G43" s="2">
+        <f t="shared" si="0"/>
+        <v>4.8306930693069308E-2</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="1"/>
+        <v>0.62799009900990099</v>
+      </c>
+    </row>
+    <row r="44" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F44" s="2">
+        <v>288</v>
+      </c>
+      <c r="G44" s="2">
+        <f t="shared" si="0"/>
+        <v>4.847524752475247E-2</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="1"/>
+        <v>0.63017821782178218</v>
+      </c>
+    </row>
+    <row r="45" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F45" s="2">
+        <v>289</v>
+      </c>
+      <c r="G45" s="2">
+        <f t="shared" si="0"/>
+        <v>4.8643564356435638E-2</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" si="1"/>
+        <v>0.63236633663366337</v>
+      </c>
+    </row>
+    <row r="46" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F46" s="2">
+        <v>290</v>
+      </c>
+      <c r="G46" s="2">
+        <f t="shared" si="0"/>
+        <v>4.8811881188118814E-2</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="1"/>
+        <v>0.63455445544554456</v>
+      </c>
+    </row>
+    <row r="47" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F47" s="2">
+        <v>291</v>
+      </c>
+      <c r="G47" s="2">
+        <f t="shared" si="0"/>
+        <v>4.8980198019801975E-2</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" si="1"/>
+        <v>0.63674257425742575</v>
+      </c>
+    </row>
+    <row r="48" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F48" s="2">
+        <v>292</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="0"/>
+        <v>4.9148514851485144E-2</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="1"/>
+        <v>0.63893069306930694</v>
+      </c>
+    </row>
+    <row r="49" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F49" s="2">
+        <v>293</v>
+      </c>
+      <c r="G49" s="2">
+        <f t="shared" si="0"/>
+        <v>4.9316831683168319E-2</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="1"/>
+        <v>0.64111881188118813</v>
+      </c>
+    </row>
+    <row r="50" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F50" s="2">
+        <v>294</v>
+      </c>
+      <c r="G50" s="2">
+        <f t="shared" si="0"/>
+        <v>4.9485148514851481E-2</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="1"/>
+        <v>0.64330693069306932</v>
+      </c>
+    </row>
+    <row r="51" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F51" s="2">
+        <v>295</v>
+      </c>
+      <c r="G51" s="2">
+        <f t="shared" si="0"/>
+        <v>4.9653465346534649E-2</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="1"/>
+        <v>0.64549504950495051</v>
+      </c>
+    </row>
+    <row r="52" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F52" s="2">
+        <v>296</v>
+      </c>
+      <c r="G52" s="2">
+        <f t="shared" si="0"/>
+        <v>4.9821782178217824E-2</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="1"/>
+        <v>0.6476831683168317</v>
+      </c>
+    </row>
+    <row r="53" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F53" s="2">
+        <v>297</v>
+      </c>
+      <c r="G53" s="2">
+        <f t="shared" si="0"/>
+        <v>4.9990099009900986E-2</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="1"/>
+        <v>0.64987128712871289</v>
+      </c>
+    </row>
+    <row r="54" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F54" s="2">
+        <v>298</v>
+      </c>
+      <c r="G54" s="2">
+        <f t="shared" si="0"/>
+        <v>5.0158415841584154E-2</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="1"/>
+        <v>0.65205940594059408</v>
+      </c>
+    </row>
+    <row r="55" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F55" s="2">
+        <v>299</v>
+      </c>
+      <c r="G55" s="2">
+        <f t="shared" si="0"/>
+        <v>5.0326732673267323E-2</v>
+      </c>
+      <c r="H55" s="2">
+        <f t="shared" si="1"/>
+        <v>0.65424752475247527</v>
+      </c>
+    </row>
+    <row r="56" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F56" s="2">
+        <v>300</v>
+      </c>
+      <c r="G56" s="2">
+        <f t="shared" si="0"/>
+        <v>5.0495049504950491E-2</v>
+      </c>
+      <c r="H56" s="2">
+        <f t="shared" si="1"/>
+        <v>0.65643564356435646</v>
+      </c>
+    </row>
+    <row r="57" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F57" s="2">
+        <v>301</v>
+      </c>
+      <c r="G57" s="2">
+        <f t="shared" si="0"/>
+        <v>5.066336633663366E-2</v>
+      </c>
+      <c r="H57" s="2">
+        <f t="shared" si="1"/>
+        <v>0.65862376237623765</v>
+      </c>
+    </row>
+    <row r="58" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F58" s="2">
+        <v>302</v>
+      </c>
+      <c r="G58" s="2">
+        <f t="shared" si="0"/>
+        <v>5.0831683168316828E-2</v>
+      </c>
+      <c r="H58" s="2">
+        <f t="shared" si="1"/>
+        <v>0.66081188118811884</v>
+      </c>
+    </row>
+    <row r="59" spans="6:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="F59" s="2">
+        <v>303</v>
+      </c>
+      <c r="G59" s="1">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="H59" s="1">
+        <v>0.66300000000000003</v>
+      </c>
+    </row>
+    <row r="76" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P76" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD56995-6286-4A66-83F4-08892FD4F382}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>